<commit_message>
Update RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2020.xlsx
</commit_message>
<xml_diff>
--- a/testes_planilhas/RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2020.xlsx
+++ b/testes_planilhas/RELATÓRIO DE DESFAZIMENTO DE BENS MÓVEIS PATRIMONIAIS DE 2020.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sap_ufac_meta" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -443,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,8 +513,10 @@
       <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>100100</v>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>100100</t>
+        </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
@@ -552,8 +553,10 @@
       <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>100101</v>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>100101</t>
+        </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
@@ -590,8 +593,10 @@
       <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>100102</v>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>100102</t>
+        </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
@@ -628,8 +633,10 @@
       <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>100103</v>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>100103</t>
+        </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
@@ -657,6 +664,126 @@
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>100104</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Projetor Multimídia Epson PowerLite S41+</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>10/01/2023</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 51234</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Centro de Educação, Letras e Artes (CELA)</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>100105</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Ar-condicionado Split 12.000 BTUs, Springer Midea</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>05/09/2020</t>
+        </is>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 20556</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Coordenação do Curso de Sistemas de Informação</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>Alienação/Leilão</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>100106</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>Impressora a Laser HP LaserJet Pro M130fw</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>22/05/2022</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
+        <is>
+          <t>NF-e 47890</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Pró-Reitoria de Desenvolvimento e Gestão de Pessoas (PRODGEP)</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>Irrecuperável</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
         <is>
           <t>Alienação/Leilão</t>
         </is>
@@ -668,33 +795,4 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id_desfazimento</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>